<commit_message>
another unnecessarily large change
</commit_message>
<xml_diff>
--- a/src/test/resources/files/testdata.xlsx
+++ b/src/test/resources/files/testdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kamil.nowocin/Desktop/Test_Automation-automationpractice/src/test/resources/files/"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="11">
   <si>
     <t>wwww@test.pl</t>
   </si>
@@ -49,11 +49,30 @@
   <si>
     <t>STATUS</t>
   </si>
+  <si>
+    <t>FAILED</t>
+  </si>
+  <si>
+    <t>PASSED</t>
+  </si>
+  <si>
+    <t>Subscribe to Newsletter on Freemium Websites</t>
+  </si>
+  <si>
+    <t>SUBSCRIBE TO NEWSLETTER ON FREEMIUM WEBSITES</t>
+  </si>
+  <si>
+    <t>AS A USER I WOULD LIKE TO CHECK AVAILABILITY OF MY EMAIL ADDRESS</t>
+  </si>
+  <si>
+    <t>Subscribe to Newsletter on Selectives Websites</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="12"/>
@@ -529,7 +548,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3948BB33-7707-DB4E-B60C-146BE6C8A78E}">
-  <dimension ref="A1:Z99"/>
+  <dimension ref="A1:I99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -538,22 +557,22 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="7" width="10.83203125" style="1" collapsed="1"/>
-    <col min="8" max="9" width="10.83203125" style="2" collapsed="1"/>
-    <col min="14" max="17" width="10.83203125" style="1" collapsed="1"/>
-    <col min="22" max="22" width="10.83203125" style="1" collapsed="1"/>
-    <col min="27" max="16384" width="10.83203125" style="1" collapsed="1"/>
+    <col min="1" max="7" style="1" width="10.83203125" collapsed="true"/>
+    <col min="8" max="9" style="2" width="10.83203125" collapsed="true"/>
+    <col min="14" max="17" style="1" width="10.83203125" collapsed="true"/>
+    <col min="22" max="22" style="1" width="10.83203125" collapsed="true"/>
+    <col min="27" max="16384" style="1" width="10.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="7" customFormat="1" ht="17" thickBot="1">
       <c r="A1" s="13" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
       <c r="E1" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>2</v>
@@ -565,11 +584,15 @@
       <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:9" s="3" customFormat="1" ht="17" thickBot="1">
-      <c r="A2" s="14"/>
+      <c r="A2" s="14" t="s">
+        <v>10</v>
+      </c>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
-      <c r="E2" s="5"/>
+      <c r="E2" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="F2" s="15" t="s">
         <v>0</v>
       </c>
@@ -580,11 +603,15 @@
       <c r="I2" s="12"/>
     </row>
     <row r="3" spans="1:9" s="3" customFormat="1" ht="17" thickBot="1">
-      <c r="A3" s="8"/>
+      <c r="A3" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
-      <c r="E3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
       <c r="H3" s="10"/>
@@ -1053,11 +1080,15 @@
       <c r="I45" s="10"/>
     </row>
     <row r="46" spans="1:9" ht="17" thickBot="1">
-      <c r="A46" s="8"/>
+      <c r="A46" s="8" t="s">
+        <v>9</v>
+      </c>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
-      <c r="E46" s="4"/>
+      <c r="E46" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="F46" s="9"/>
       <c r="G46" s="9"/>
       <c r="H46" s="10"/>

</xml_diff>

<commit_message>
feat/added github action for gradle-clean-test
</commit_message>
<xml_diff>
--- a/src/test/resources/files/testdata.xlsx
+++ b/src/test/resources/files/testdata.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="11">
   <si>
     <t>wwww@test.pl</t>
   </si>
@@ -591,7 +591,7 @@
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
       <c r="E2" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F2" s="15" t="s">
         <v>0</v>
@@ -610,7 +610,7 @@
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
       <c r="E3" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>

</xml_diff>

<commit_message>
chore/changed back to gradlew
</commit_message>
<xml_diff>
--- a/src/test/resources/files/testdata.xlsx
+++ b/src/test/resources/files/testdata.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="11">
   <si>
     <t>wwww@test.pl</t>
   </si>
@@ -1081,13 +1081,13 @@
     </row>
     <row r="46" spans="1:9" ht="17" thickBot="1">
       <c r="A46" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
       <c r="E46" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F46" s="9"/>
       <c r="G46" s="9"/>

</xml_diff>